<commit_message>
Adds map-coloring of scheduled boats
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ESS\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ESS\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863A98C7-5D01-4C3E-9BC4-3546773FDC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD3C47C-E9F6-43D1-A693-FC94F4428EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18555" windowHeight="16500" xr2:uid="{B998FFB9-F4D4-4C8B-8B91-39A2F1922F55}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="37920" xr2:uid="{B998FFB9-F4D4-4C8B-8B91-39A2F1922F55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,14 +239,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -258,9 +257,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -271,12 +267,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,12 +592,12 @@
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" style="5" customWidth="1"/>
@@ -625,7 +616,7 @@
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="14"/>
+      <c r="D1" s="12"/>
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
@@ -634,91 +625,93 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
-    <row r="4" spans="1:24" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:24" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I4"/>
-      <c r="J4" s="7"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
+      <c r="J4" s="6"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I5" s="13"/>
+    <row r="5" spans="1:24" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="18"/>
+      <c r="I5"/>
+      <c r="J5" s="6"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
     </row>
-    <row r="6" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="6"/>
-      <c r="F6"/>
-      <c r="G6" s="9"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I7" s="13"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="I8" s="13"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="I8" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A6:B6"/>
-  </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>